<commit_message>
login ddt tests are done
</commit_message>
<xml_diff>
--- a/src/test/resources/DemoblazeTestData.xlsx
+++ b/src/test/resources/DemoblazeTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umranerdogan/IdeaProjects/MyAutomationProject/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D088A78D-EC07-1F4F-B197-B3A4741F82A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988C8C0A-83BD-5A4D-A2E1-B571ADC3E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00BBB604-75EF-4AAC-AC68-8F338E48E10F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>asdfgfdsa</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -440,12 +443,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>

</xml_diff>